<commit_message>
:sparkles: Add rebel() and rebel_sheet() with tests and man
</commit_message>
<xml_diff>
--- a/tests/testthat/merged.xlsx
+++ b/tests/testthat/merged.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1120" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="226">
   <si>
     <t>A1</t>
   </si>
@@ -495,6 +496,216 @@
   </si>
   <si>
     <t>H23</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>A25</t>
+  </si>
+  <si>
+    <t>A26</t>
+  </si>
+  <si>
+    <t>A27</t>
+  </si>
+  <si>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>A29</t>
+  </si>
+  <si>
+    <t>A30</t>
+  </si>
+  <si>
+    <t>A31</t>
+  </si>
+  <si>
+    <t>A32</t>
+  </si>
+  <si>
+    <t>A33</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>E24</t>
+  </si>
+  <si>
+    <t>E25</t>
+  </si>
+  <si>
+    <t>E26</t>
+  </si>
+  <si>
+    <t>E27</t>
+  </si>
+  <si>
+    <t>E28</t>
+  </si>
+  <si>
+    <t>E29</t>
+  </si>
+  <si>
+    <t>E30</t>
+  </si>
+  <si>
+    <t>E31</t>
+  </si>
+  <si>
+    <t>E32</t>
+  </si>
+  <si>
+    <t>E33</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>D25</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>D28</t>
+  </si>
+  <si>
+    <t>D29</t>
+  </si>
+  <si>
+    <t>D30</t>
+  </si>
+  <si>
+    <t>D31</t>
+  </si>
+  <si>
+    <t>D32</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>F24</t>
+  </si>
+  <si>
+    <t>F25</t>
+  </si>
+  <si>
+    <t>F26</t>
+  </si>
+  <si>
+    <t>F27</t>
+  </si>
+  <si>
+    <t>F28</t>
+  </si>
+  <si>
+    <t>F29</t>
+  </si>
+  <si>
+    <t>F30</t>
+  </si>
+  <si>
+    <t>F31</t>
+  </si>
+  <si>
+    <t>F32</t>
+  </si>
+  <si>
+    <t>F33</t>
+  </si>
+  <si>
+    <t>G24</t>
+  </si>
+  <si>
+    <t>G25</t>
+  </si>
+  <si>
+    <t>G26</t>
+  </si>
+  <si>
+    <t>G27</t>
+  </si>
+  <si>
+    <t>G28</t>
+  </si>
+  <si>
+    <t>G29</t>
+  </si>
+  <si>
+    <t>G30</t>
+  </si>
+  <si>
+    <t>G31</t>
+  </si>
+  <si>
+    <t>G32</t>
+  </si>
+  <si>
+    <t>G33</t>
+  </si>
+  <si>
+    <t>H24</t>
+  </si>
+  <si>
+    <t>H25</t>
+  </si>
+  <si>
+    <t>H26</t>
+  </si>
+  <si>
+    <t>H27</t>
+  </si>
+  <si>
+    <t>H28</t>
+  </si>
+  <si>
+    <t>H29</t>
+  </si>
+  <si>
+    <t>H30</t>
+  </si>
+  <si>
+    <t>H31</t>
+  </si>
+  <si>
+    <t>H32</t>
+  </si>
+  <si>
+    <t>H33</t>
   </si>
 </sst>
 </file>
@@ -814,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1365,6 +1576,575 @@
       </c>
       <c r="H23" t="s">
         <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" t="s">
+        <v>154</v>
+      </c>
+      <c r="H13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" t="s">
+        <v>207</v>
+      </c>
+      <c r="H15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18" t="s">
+        <v>210</v>
+      </c>
+      <c r="H18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19" t="s">
+        <v>211</v>
+      </c>
+      <c r="H19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" t="s">
+        <v>202</v>
+      </c>
+      <c r="G20" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" t="s">
+        <v>203</v>
+      </c>
+      <c r="G21" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" t="s">
+        <v>215</v>
+      </c>
+      <c r="H23" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>